<commit_message>
updated the asset code issue and image upload
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/depreciation.xlsx
+++ b/afar_project/csv_path/excel_files/depreciation.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
asset profile section updated and freed from bug
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/depreciation.xlsx
+++ b/afar_project/csv_path/excel_files/depreciation.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sl </t>
+          <t>Sl</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0001</t>
+          <t>FRC-HQ-SLM-O-2017-0001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -873,7 +873,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0002</t>
+          <t>FRC-HQ-SLM-O-2017-0002</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0003</t>
+          <t>FRC-HQ-SLM-O-2017-0003</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0005</t>
+          <t>FRC-HQ-SLM-O-2017-0005</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0006</t>
+          <t>FRC-HQ-SLM-O-2017-0006</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0007</t>
+          <t>FRC-HQ-SLM-O-2017-0007</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0008</t>
+          <t>FRC-HQ-SLM-O-2017-0008</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0009</t>
+          <t>FRC-HQ-SLM-O-2017-0009</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0010</t>
+          <t>FRC-HQ-SLM-C-2017-0010</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0011</t>
+          <t>FRC-HQ-SLM-C-2017-0011</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0012</t>
+          <t>FRC-HQ-SLM-O-2017-0012</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0013</t>
+          <t>FRC-HQ-SLM-O-2017-0013</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0014</t>
+          <t>FRC-HQ-SLM-F-2017-0014</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0015</t>
+          <t>FRC-HQ-SLM-O-2017-0015</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0016</t>
+          <t>FRC-HQ-SLM-O-2017-0016</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0017</t>
+          <t>FRC-HQ-SLM-F-2017-0017</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0018</t>
+          <t>FRC-HQ-SLM-O-2017-0018</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0019</t>
+          <t>FRC-HQ-SLM-F-2017-0019</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0020</t>
+          <t>FRC-HQ-SLM-F-2017-0020</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0021</t>
+          <t>FRC-HQ-SLM-O-2017-0021</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0022</t>
+          <t>FRC-HQ-SLM-O-2017-0022</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0023</t>
+          <t>FRC-HQ-SLM-O-2017-0023</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0024</t>
+          <t>FRC-HQ-SLM-F-2017-0024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0025</t>
+          <t>FRC-HQ-SLM-F-2017-0025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0026</t>
+          <t>FRC-HQ-SLM-F-2017-0026</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0027</t>
+          <t>FRC-HQ-SLM-F-2017-0027</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0028</t>
+          <t>FRC-HQ-SLM-O-2017-0028</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0029</t>
+          <t>FRC-HQ-SLM-F-2017-0029</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0030</t>
+          <t>FRC-HQ-SLM-F-2017-0030</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -5773,7 +5773,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0031</t>
+          <t>FRC-HQ-SLM-F-2017-0031</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -5948,7 +5948,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0032</t>
+          <t>FRC-HQ-SLM-O-2017-0032</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -6123,7 +6123,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0033</t>
+          <t>FRC-HQ-SLM-F-2017-0033</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -6298,7 +6298,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0034</t>
+          <t>FRC-HQ-SLM-O-2017-0034</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0035</t>
+          <t>FRC-HQ-SLM-F-2017-0035</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -6648,7 +6648,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0036</t>
+          <t>FRC-HQ-SLM-O-2017-0036</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -6823,7 +6823,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0037</t>
+          <t>FRC-HQ-SLM-O-2017-0037</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -6998,7 +6998,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0038</t>
+          <t>FRC-HQ-SLM-O-2017-0038</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -7173,7 +7173,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0039</t>
+          <t>FRC-HQ-SLM-F-2017-0039</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0040</t>
+          <t>FRC-HQ-SLM-F-2017-0040</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0041</t>
+          <t>FRC-HQ-SLM-O-2017-0041</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -7698,7 +7698,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0042</t>
+          <t>FRC-HQ-SLM-F-2017-0042</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -7873,7 +7873,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0043</t>
+          <t>FRC-HQ-SLM-F-2017-0043</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -8048,7 +8048,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0044</t>
+          <t>FRC-HQ-SLM-F-2017-0044</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -8223,7 +8223,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-17-0045</t>
+          <t>FRC-HQ-SLM-T-2017-0045</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -8398,7 +8398,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-17-0046</t>
+          <t>FRC-HQ-SLM-T-2017-0046</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -8573,7 +8573,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0047</t>
+          <t>FRC-HQ-SLM-F-2017-0047</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0048</t>
+          <t>FRC-HQ-SLM-O-2017-0048</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -8923,7 +8923,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0049</t>
+          <t>FRC-HQ-SLM-F-2017-0049</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -9098,7 +9098,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0050</t>
+          <t>FRC-HQ-SLM-O-2017-0050</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -9273,7 +9273,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0051</t>
+          <t>FRC-HQ-SLM-O-2017-0051</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -9448,7 +9448,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0052</t>
+          <t>FRC-HQ-SLM-F-2017-0052</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -9623,7 +9623,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0053</t>
+          <t>FRC-HQ-SLM-F-2017-0053</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -9798,7 +9798,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0054</t>
+          <t>FRC-HQ-SLM-F-2018-0054</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -9973,7 +9973,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0055</t>
+          <t>FRC-HQ-SLM-F-2018-0055</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -10148,7 +10148,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0056</t>
+          <t>FRC-HQ-SLM-F-2018-0056</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -10323,7 +10323,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0057</t>
+          <t>FRC-HQ-SLM-F-2018-0057</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -10498,7 +10498,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0058</t>
+          <t>FRC-HQ-SLM-F-2018-0058</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -10673,7 +10673,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0059</t>
+          <t>FRC-HQ-SLM-F-2018-0059</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -10848,7 +10848,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0060</t>
+          <t>FRC-HQ-SLM-C-2018-0060</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -11023,7 +11023,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0061</t>
+          <t>FRC-HQ-SLM-C-2018-0061</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0062</t>
+          <t>FRC-HQ-SLM-O-2018-0062</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -11373,7 +11373,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0063</t>
+          <t>FRC-HQ-SLM-F-2018-0063</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -11548,7 +11548,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0064</t>
+          <t>FRC-HQ-SLM-F-2018-0064</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0065</t>
+          <t>FRC-HQ-SLM-C-2018-0065</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0066</t>
+          <t>FRC-HQ-SLM-C-2018-0066</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -12073,7 +12073,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0067</t>
+          <t>FRC-HQ-SLM-F-2018-0067</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -12248,7 +12248,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0068</t>
+          <t>FRC-HQ-SLM-F-2018-0068</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -12423,7 +12423,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0069</t>
+          <t>FRC-HQ-SLM-F-2018-0069</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0070</t>
+          <t>FRC-HQ-SLM-F-2018-0070</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -12773,7 +12773,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0071</t>
+          <t>FRC-HQ-SLM-C-2018-0071</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -12948,7 +12948,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0072</t>
+          <t>FRC-HQ-SLM-F-2018-0072</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -13123,7 +13123,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0073</t>
+          <t>FRC-HQ-SLM-F-2018-0073</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -13298,7 +13298,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0074</t>
+          <t>FRC-HQ-SLM-F-2018-0074</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -13473,7 +13473,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0075</t>
+          <t>FRC-HQ-SLM-F-2018-0075</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -13648,7 +13648,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0076</t>
+          <t>FRC-HQ-SLM-T-2018-0076</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -13823,7 +13823,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0077</t>
+          <t>FRC-HQ-SLM-F-2018-0077</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -13998,7 +13998,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0078</t>
+          <t>FRC-HQ-SLM-F-2018-0078</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -14173,7 +14173,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0079</t>
+          <t>FRC-HQ-SLM-F-2018-0079</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -14348,7 +14348,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0080</t>
+          <t>FRC-HQ-SLM-C-2018-0080</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -14523,7 +14523,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0081</t>
+          <t>FRC-HQ-SLM-C-2018-0081</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -14698,7 +14698,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0082</t>
+          <t>FRC-HQ-SLM-C-2018-0082</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -14873,7 +14873,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0083</t>
+          <t>FRC-HQ-SLM-C-2018-0083</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -15048,7 +15048,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0084</t>
+          <t>FRC-HQ-SLM-O-2018-0084</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -15223,7 +15223,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0085</t>
+          <t>FRC-HQ-SLM-C-2018-0085</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -15398,7 +15398,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0086</t>
+          <t>FRC-HQ-SLM-C-2018-0086</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -15573,7 +15573,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0087</t>
+          <t>FRC-HQ-SLM-O-2018-0087</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -15748,7 +15748,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0088</t>
+          <t>FRC-HQ-SLM-C-2018-0088</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -15923,7 +15923,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0089</t>
+          <t>FRC-HQ-SLM-C-2018-0089</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -16098,7 +16098,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0090</t>
+          <t>FRC-HQ-SLM-C-2018-0090</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -16273,7 +16273,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0091</t>
+          <t>FRC-HQ-SLM-F-2018-0091</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -16448,7 +16448,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0092</t>
+          <t>FRC-HQ-SLM-F-2018-0092</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -16623,7 +16623,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0093</t>
+          <t>FRC-HQ-SLM-F-2018-0093</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -16798,7 +16798,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0094</t>
+          <t>FRC-HQ-SLM-O-2018-0094</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -16973,7 +16973,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0095</t>
+          <t>FRC-HQ-SLM-F-2018-0095</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -17148,7 +17148,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0096</t>
+          <t>FRC-HQ-SLM-O-2018-0096</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -17323,7 +17323,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0097</t>
+          <t>FRC-HQ-SLM-T-2018-0097</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -17498,7 +17498,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-18-0098</t>
+          <t>FRC-HQ-SLM-M-2018-0098</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -17673,7 +17673,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-18-0099</t>
+          <t>FRC-HQ-SLM-M-2018-0099</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -17848,7 +17848,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0100</t>
+          <t>FRC-HQ-SLM-O-2018-0100</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -18023,7 +18023,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0101</t>
+          <t>FRC-HQ-SLM-O-2018-0101</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -18198,7 +18198,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0102</t>
+          <t>FRC-HQ-SLM-O-2018-0102</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -18373,7 +18373,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0103</t>
+          <t>FRC-HQ-SLM-O-2018-0103</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -18548,7 +18548,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0104</t>
+          <t>FRC-HQ-SLM-O-2018-0104</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -18723,7 +18723,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0105</t>
+          <t>FRC-HQ-SLM-O-2018-0105</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -18898,7 +18898,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0106</t>
+          <t>FRC-HQ-SLM-O-2018-0106</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -19073,7 +19073,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0107</t>
+          <t>FRC-HQ-SLM-O-2018-0107</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -19248,7 +19248,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0108</t>
+          <t>FRC-HQ-SLM-O-2018-0108</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -19423,7 +19423,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0109</t>
+          <t>FRC-HQ-SLM-O-2018-0109</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -19598,7 +19598,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0110</t>
+          <t>FRC-HQ-SLM-F-2018-0110</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -19773,7 +19773,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0111</t>
+          <t>FRC-HQ-SLM-F-2019-0111</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -19948,7 +19948,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0112</t>
+          <t>FRC-HQ-SLM-F-2019-0112</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -20123,7 +20123,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0113</t>
+          <t>FRC-HQ-SLM-F-2019-0113</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -20298,7 +20298,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0114</t>
+          <t>FRC-HQ-SLM-F-2019-0114</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -20473,7 +20473,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0115</t>
+          <t>FRC-HQ-SLM-F-2019-0115</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -20648,7 +20648,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0116</t>
+          <t>FRC-HQ-SLM-O-2019-0116</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -20823,7 +20823,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0117</t>
+          <t>FRC-HQ-SLM-F-2019-0117</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -20998,7 +20998,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0118</t>
+          <t>FRC-HQ-SLM-F-2019-0118</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -21173,7 +21173,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0119</t>
+          <t>FRC-HQ-SLM-O-2019-0119</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -21348,7 +21348,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0120</t>
+          <t>FRC-HQ-SLM-O-2019-0120</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -21523,7 +21523,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0121</t>
+          <t>FRC-HQ-SLM-F-2019-0121</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -21698,7 +21698,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0122</t>
+          <t>FRC-HQ-SLM-C-2019-0122</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -21873,7 +21873,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0123</t>
+          <t>FRC-HQ-SLM-C-2019-0123</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -22048,7 +22048,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0124</t>
+          <t>FRC-HQ-SLM-C-2019-0124</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -22223,7 +22223,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0125</t>
+          <t>FRC-HQ-SLM-C-2019-0125</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -22398,7 +22398,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0126</t>
+          <t>FRC-HQ-SLM-F-2019-0126</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -22573,7 +22573,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0127</t>
+          <t>FRC-HQ-SLM-F-2019-0127</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -22748,7 +22748,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0128</t>
+          <t>FRC-HQ-SLM-F-2019-0128</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -22923,7 +22923,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0129</t>
+          <t>FRC-HQ-SLM-C-2020-0129</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -23098,7 +23098,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0130</t>
+          <t>FRC-HQ-SLM-C-2020-0130</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -23273,7 +23273,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0131</t>
+          <t>FRC-HQ-SLM-C-2020-0131</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -23448,7 +23448,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0132</t>
+          <t>FRC-HQ-SLM-C-2020-0132</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -23623,7 +23623,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-20-0133</t>
+          <t>FRC-HQ-SLM-T-2020-0133</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -23798,7 +23798,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0134</t>
+          <t>FRC-HQ-SLM-C-2020-0134</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -23973,7 +23973,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0135</t>
+          <t>FRC-HQ-SLM-C-2020-0135</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -24148,7 +24148,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0136</t>
+          <t>FRC-HQ-SLM-C-2020-0136</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -24323,7 +24323,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0137</t>
+          <t>FRC-HQ-SLM-C-2020-0137</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -24498,7 +24498,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0138</t>
+          <t>FRC-HQ-SLM-F-2020-0138</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -24673,7 +24673,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0139</t>
+          <t>FRC-HQ-SLM-C-2020-0139</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -24848,7 +24848,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0140</t>
+          <t>FRC-HQ-SLM-F-2020-0140</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -25023,7 +25023,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0141</t>
+          <t>FRC-HQ-SLM-C-2020-0141</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -25198,7 +25198,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0142</t>
+          <t>FRC-HQ-SLM-C-2020-0142</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -25373,7 +25373,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0143</t>
+          <t>FRC-HQ-SLM-M-2021-0143</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -25548,7 +25548,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0144</t>
+          <t>FRC-HQ-SLM-M-2021-0144</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -25723,7 +25723,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-21-0145</t>
+          <t>FRC-HQ-SLM-O-2021-0145</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -25898,7 +25898,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0146</t>
+          <t>FRC-HQ-SLM-C-2021-0146</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -26073,7 +26073,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0147</t>
+          <t>FRC-HQ-SLM-C-2021-0147</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -26248,7 +26248,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0148</t>
+          <t>FRC-HQ-SLM-M-2021-0148</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -26423,7 +26423,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0149</t>
+          <t>FRC-HQ-SLM-F-2021-0149</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-21-0150</t>
+          <t>FRC-HQ-SLM-O-2021-0150</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -26773,7 +26773,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0152</t>
+          <t>FRC-HQ-SLM-C-2021-0152</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -26948,7 +26948,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0153</t>
+          <t>FRC-HQ-SLM-C-2021-0153</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -27123,7 +27123,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0154</t>
+          <t>FRC-HQ-SLM-C-2021-0154</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -27298,7 +27298,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0155</t>
+          <t>FRC-HQ-SLM-C-2021-0155</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -27473,7 +27473,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0156</t>
+          <t>FRC-HQ-SLM-C-2021-0156</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -27648,7 +27648,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0157</t>
+          <t>FRC-HQ-SLM-C-2021-0157</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -27823,7 +27823,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0158</t>
+          <t>FRC-HQ-SLM-C-2021-0158</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -27998,7 +27998,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0159</t>
+          <t>FRC-HQ-SLM-C-2021-0159</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -28173,7 +28173,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0160</t>
+          <t>FRC-HQ-SLM-C-2021-0160</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -28348,7 +28348,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0161</t>
+          <t>FRC-HQ-SLM-C-2021-0161</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -28523,7 +28523,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0162</t>
+          <t>FRC-HQ-SLM-I-2021-0162</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -28698,7 +28698,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0163</t>
+          <t>FRC-HQ-SLM-I-2021-0163</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -28873,7 +28873,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0164</t>
+          <t>FRC-HQ-SLM-I-2021-0164</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -29048,7 +29048,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0165</t>
+          <t>FRC-HQ-SLM-I-2021-0165</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -29223,7 +29223,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0166</t>
+          <t>FRC-HQ-SLM-I-2021-0166</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -29398,7 +29398,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0167</t>
+          <t>FRC-HQ-SLM-I-2021-0167</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -29573,7 +29573,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0168</t>
+          <t>FRC-HQ-SLM-I-2021-0168</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -29748,7 +29748,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0169</t>
+          <t>FRC-HQ-SLM-I-2021-0169</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -29924,7 +29924,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0170</t>
+          <t>FRC-HQ-SLM-I-2021-0170</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -30099,7 +30099,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0171</t>
+          <t>FRC-HQ-SLM-I-2021-0171</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -30274,7 +30274,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0172</t>
+          <t>FRC-HQ-SLM-I-2021-0172</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -30449,7 +30449,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0173</t>
+          <t>FRC-HQ-SLM-S-2021-0173</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -30624,7 +30624,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0174</t>
+          <t>FRC-HQ-SLM-S-2021-0174</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -30799,7 +30799,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0175</t>
+          <t>FRC-HQ-SLM-S-2021-0175</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -30974,7 +30974,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0176</t>
+          <t>FRC-HQ-SLM-S-2021-0176</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -31149,7 +31149,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0177</t>
+          <t>FRC-HQ-SLM-S-2021-0177</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -31324,7 +31324,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0178</t>
+          <t>FRC-HQ-SLM-S-2021-0178</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -31499,7 +31499,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0179</t>
+          <t>FRC-HQ-SLM-S-2021-0179</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -31674,7 +31674,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0180</t>
+          <t>FRC-HQ-SLM-S-2021-0180</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -31849,7 +31849,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0181</t>
+          <t>FRC-HQ-SLM-S-2021-0181</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -32024,7 +32024,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0182</t>
+          <t>FRC-HQ-SLM-S-2021-0182</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -32199,7 +32199,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0183</t>
+          <t>FRC-HQ-SLM-S-2021-0183</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -32374,7 +32374,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0184</t>
+          <t>FRC-HQ-SLM-S-2021-0184</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -32550,7 +32550,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0185</t>
+          <t>FRC-HQ-SLM-S-2021-0185</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -32725,7 +32725,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0186</t>
+          <t>FRC-HQ-SLM-S-2021-0186</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -32900,7 +32900,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0187</t>
+          <t>FRC-HQ-SLM-S-2021-0187</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -33075,7 +33075,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0188</t>
+          <t>FRC-HQ-SLM-S-2021-0188</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -33250,7 +33250,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0189</t>
+          <t>FRC-HQ-SLM-S-2021-0189</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -33425,7 +33425,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0190</t>
+          <t>FRC-HQ-SLM-S-2021-0190</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -33600,7 +33600,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0191</t>
+          <t>FRC-HQ-SLM-S-2021-0191</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -33775,7 +33775,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0192</t>
+          <t>FRC-HQ-SLM-S-2021-0192</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -33950,7 +33950,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0193</t>
+          <t>FRC-HQ-SLM-S-2021-0193</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -34125,7 +34125,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0194</t>
+          <t>FRC-HQ-SLM-S-2021-0194</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -34300,7 +34300,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0195</t>
+          <t>FRC-HQ-SLM-S-2021-0195</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -34475,7 +34475,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0196</t>
+          <t>FRC-HQ-SLM-S-2021-0196</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -34650,7 +34650,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0197</t>
+          <t>FRC-HQ-SLM-S-2021-0197</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -34825,7 +34825,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0198</t>
+          <t>FRC-HQ-SLM-E-2021-0198</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -35000,7 +35000,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0199</t>
+          <t>FRC-HQ-SLM-E-2021-0199</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -35175,7 +35175,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0200</t>
+          <t>FRC-HQ-SLM-E-2021-0200</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -35350,7 +35350,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0201</t>
+          <t>FRC-HQ-SLM-E-2021-0201</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -35525,7 +35525,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0202</t>
+          <t>FRC-HQ-SLM-E-2021-0202</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -35700,7 +35700,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0203</t>
+          <t>FRC-HQ-SLM-E-2021-0203</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -35875,7 +35875,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0204</t>
+          <t>FRC-HQ-SLM-E-2021-0204</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -36050,7 +36050,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0205</t>
+          <t>FRC-HQ-SLM-E-2021-0205</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -36225,7 +36225,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0206</t>
+          <t>FRC-HQ-SLM-E-2021-0206</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -36400,7 +36400,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0207</t>
+          <t>FRC-HQ-SLM-E-2021-0207</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -36575,7 +36575,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0208</t>
+          <t>FRC-HQ-SLM-E-2021-0208</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -36750,7 +36750,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0209</t>
+          <t>FRC-HQ-SLM-E-2021-0209</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -36925,7 +36925,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0210</t>
+          <t>FRC-HQ-SLM-E-2021-0210</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -37100,7 +37100,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0211</t>
+          <t>FRC-HQ-SLM-E-2021-0211</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -37275,7 +37275,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0212</t>
+          <t>FRC-HQ-SLM-E-2021-0212</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -37450,7 +37450,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0213</t>
+          <t>FRC-HQ-SLM-E-2021-0213</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -37625,7 +37625,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0214</t>
+          <t>FRC-HQ-SLM-E-2021-0214</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -37800,7 +37800,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0215</t>
+          <t>FRC-HQ-SLM-E-2021-0215</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -37975,7 +37975,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0216</t>
+          <t>FRC-HQ-SLM-E-2021-0216</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -38150,7 +38150,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0217</t>
+          <t>FRC-HQ-SLM-E-2021-0217</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -38325,7 +38325,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0218</t>
+          <t>FRC-HQ-SLM-E-2021-0218</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -38500,7 +38500,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0219</t>
+          <t>FRC-HQ-SLM-E-2021-0219</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -38675,7 +38675,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0220</t>
+          <t>FRC-HQ-SLM-E-2021-0220</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -38850,7 +38850,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0221</t>
+          <t>FRC-HQ-SLM-E-2021-0221</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -39025,7 +39025,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0222</t>
+          <t>FRC-HQ-SLM-E-2021-0222</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -39200,7 +39200,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0223</t>
+          <t>FRC-HQ-SLM-E-2021-0223</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -39375,7 +39375,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0224</t>
+          <t>FRC-HQ-SLM-E-2021-0224</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -39550,7 +39550,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0225</t>
+          <t>FRC-HQ-SLM-E-2021-0225</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -39725,7 +39725,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0226</t>
+          <t>FRC-HQ-SLM-E-2021-0226</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -39900,7 +39900,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0227</t>
+          <t>FRC-HQ-SLM-E-2021-0227</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -40075,7 +40075,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0228</t>
+          <t>FRC-HQ-SLM-E-2021-0228</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -40250,7 +40250,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0229</t>
+          <t>FRC-HQ-SLM-E-2021-0229</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -40425,7 +40425,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0230</t>
+          <t>FRC-HQ-SLM-E-2021-0230</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -40600,7 +40600,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0231</t>
+          <t>FRC-HQ-SLM-E-2021-0231</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -40775,7 +40775,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0232</t>
+          <t>FRC-HQ-SLM-E-2021-0232</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -40950,7 +40950,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0233</t>
+          <t>FRC-HQ-SLM-E-2021-0233</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -41125,7 +41125,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0234</t>
+          <t>FRC-HQ-SLM-E-2021-0234</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -41300,7 +41300,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0235</t>
+          <t>FRC-HQ-SLM-E-2021-0235</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -41475,7 +41475,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0236</t>
+          <t>FRC-HQ-SLM-E-2021-0236</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -41650,7 +41650,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0237</t>
+          <t>FRC-HQ-SLM-P-2021-0237</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -41825,7 +41825,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0238</t>
+          <t>FRC-HQ-SLM-P-2021-0238</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -42000,7 +42000,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0239</t>
+          <t>FRC-HQ-SLM-P-2021-0239</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -42175,7 +42175,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0240</t>
+          <t>FRC-HQ-SLM-P-2021-0240</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -42350,7 +42350,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0241</t>
+          <t>FRC-HQ-SLM-P-2021-0241</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -42525,7 +42525,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0242</t>
+          <t>FRC-HQ-SLM-I-2021-0242</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -42700,7 +42700,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0243</t>
+          <t>FRC-HQ-SLM-I-2021-0243</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -42875,7 +42875,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0244</t>
+          <t>FRC-HQ-SLM-I-2021-0244</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -43050,7 +43050,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0245</t>
+          <t>FRC-HQ-SLM-I-2021-0245</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -43225,7 +43225,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0246</t>
+          <t>FRC-HQ-SLM-I-2021-0246</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -43400,7 +43400,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0247</t>
+          <t>FRC-HQ-SLM-I-2021-0247</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -43575,7 +43575,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0248</t>
+          <t>FRC-HQ-SLM-I-2021-0248</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -43750,7 +43750,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0249</t>
+          <t>FRC-HQ-SLM-I-2021-0249</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -43925,7 +43925,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0250</t>
+          <t>FRC-HQ-SLM-I-2021-0250</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -44100,7 +44100,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0251</t>
+          <t>FRC-HQ-SLM-I-2021-0251</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -44275,7 +44275,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0252</t>
+          <t>FRC-HQ-SLM-I-2021-0252</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -44450,7 +44450,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0253</t>
+          <t>FRC-HQ-SLM-I-2021-0253</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -44625,7 +44625,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0254</t>
+          <t>FRC-HQ-SLM-I-2021-0254</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -44800,7 +44800,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0255</t>
+          <t>FRC-HQ-SLM-I-2021-0255</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -44975,7 +44975,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0256</t>
+          <t>FRC-HQ-SLM-I-2021-0256</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -45150,7 +45150,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0257</t>
+          <t>FRC-HQ-SLM-I-2021-0257</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -45325,7 +45325,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0258</t>
+          <t>FRC-HQ-SLM-I-2021-0258</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -45500,7 +45500,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0259</t>
+          <t>FRC-HQ-SLM-I-2021-0259</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -45675,7 +45675,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0260</t>
+          <t>FRC-HQ-SLM-I-2021-0260</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -45850,7 +45850,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0261</t>
+          <t>FRC-HQ-SLM-I-2021-0261</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -46025,7 +46025,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0262</t>
+          <t>FRC-HQ-SLM-I-2021-0262</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -46200,7 +46200,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0263</t>
+          <t>FRC-HQ-SLM-I-2021-0263</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -46375,7 +46375,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0264</t>
+          <t>FRC-HQ-SLM-I-2021-0264</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -46550,7 +46550,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0265</t>
+          <t>FRC-HQ-SLM-I-2021-0265</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -46725,7 +46725,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0266</t>
+          <t>FRC-HQ-SLM-I-2021-0266</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -46900,7 +46900,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0267</t>
+          <t>FRC-HQ-SLM-I-2021-0267</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -47075,7 +47075,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0268</t>
+          <t>FRC-HQ-SLM-I-2021-0268</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -47250,7 +47250,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0269</t>
+          <t>FRC-HQ-SLM-I-2021-0269</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -47425,7 +47425,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0270</t>
+          <t>FRC-HQ-SLM-I-2021-0270</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -47600,7 +47600,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0271</t>
+          <t>FRC-HQ-SLM-I-2021-0271</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -47775,7 +47775,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0272</t>
+          <t>FRC-HQ-SLM-I-2021-0272</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -47950,7 +47950,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0273</t>
+          <t>FRC-HQ-SLM-I-2021-0273</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -48125,7 +48125,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0274</t>
+          <t>FRC-HQ-SLM-I-2021-0274</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -48300,7 +48300,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0275</t>
+          <t>FRC-HQ-SLM-F-2021-0275</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -48475,7 +48475,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0276</t>
+          <t>FRC-HQ-SLM-F-2021-0276</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -48650,7 +48650,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0277</t>
+          <t>FRC-HQ-SLM-F-2021-0277</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -48825,7 +48825,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0278</t>
+          <t>FRC-HQ-SLM-F-2021-0278</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -49000,7 +49000,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0279</t>
+          <t>FRC-HQ-SLM-F-2021-0279</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -49175,7 +49175,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0280</t>
+          <t>FRC-HQ-SLM-F-2021-0280</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -49350,7 +49350,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0281</t>
+          <t>FRC-HQ-SLM-F-2021-0281</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -49525,7 +49525,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0282</t>
+          <t>FRC-HQ-SLM-F-2021-0282</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -49700,7 +49700,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0283</t>
+          <t>FRC-HQ-SLM-F-2021-0283</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -49875,7 +49875,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0284</t>
+          <t>FRC-HQ-SLM-F-2021-0284</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -50050,7 +50050,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0285</t>
+          <t>FRC-HQ-SLM-F-2021-0285</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -50225,7 +50225,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0286</t>
+          <t>FRC-HQ-SLM-F-2021-0286</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -50400,7 +50400,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0287</t>
+          <t>FRC-HQ-SLM-F-2021-0287</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -50575,7 +50575,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0288</t>
+          <t>FRC-HQ-SLM-F-2021-0288</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -50750,7 +50750,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0289</t>
+          <t>FRC-HQ-SLM-F-2021-0289</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -50925,7 +50925,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0290</t>
+          <t>FRC-HQ-SLM-F-2021-0290</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -51100,7 +51100,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0291</t>
+          <t>FRC-HQ-SLM-F-2021-0291</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -51275,7 +51275,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0292</t>
+          <t>FRC-HQ-SLM-F-2021-0292</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -51450,7 +51450,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0293</t>
+          <t>FRC-HQ-SLM-F-2021-0293</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -51625,7 +51625,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0294</t>
+          <t>FRC-HQ-SLM-F-2021-0294</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -51800,7 +51800,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0295</t>
+          <t>FRC-HQ-SLM-F-2021-0295</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -51975,7 +51975,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0296</t>
+          <t>FRC-HQ-SLM-F-2021-0296</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -52150,7 +52150,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0297</t>
+          <t>FRC-HQ-SLM-F-2021-0297</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -52325,7 +52325,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0298</t>
+          <t>FRC-HQ-SLM-F-2021-0298</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -52500,7 +52500,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0299</t>
+          <t>FRC-HQ-SLM-F-2021-0299</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -52675,7 +52675,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0300</t>
+          <t>FRC-HQ-SLM-F-2021-0300</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -52850,7 +52850,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0301</t>
+          <t>FRC-HQ-SLM-F-2021-0301</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -53025,7 +53025,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0001</t>
+          <t>FRC-HQ-SLM-F-2023-0001</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -53200,7 +53200,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0001</t>
+          <t>FRC-HQ-SLM-F-2023-0001</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -53375,7 +53375,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-2023-0002</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -53550,7 +53550,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-2023-0002</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -53725,7 +53725,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-2023-0002</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -53900,7 +53900,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-2023-0002</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -54075,7 +54075,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0003</t>
+          <t>FRC-HQ-SLM-F-2021-0003</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -54250,7 +54250,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0003</t>
+          <t>FRC-HQ-SLM-F-2021-0003</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -54425,7 +54425,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0006</t>
+          <t>FRC-HQ-SLM-O-2019-0006</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -54600,7 +54600,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0006</t>
+          <t>FRC-HQ-SLM-O-2019-0006</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -54775,7 +54775,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0006</t>
+          <t>FRC-HQ-SLM-F-2023-0006</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -54950,7 +54950,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0006</t>
+          <t>FRC-HQ-SLM-F-2023-0006</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -55125,7 +55125,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-23-0006</t>
+          <t>FRC-HQ-SLM-T-2023-0006</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -55300,7 +55300,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-23-0006</t>
+          <t>FRC-HQ-SLM-T-2023-0006</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -55475,7 +55475,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-2023-0006</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -55650,7 +55650,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-2023-0006</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -55825,7 +55825,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-2023-0006</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -56000,7 +56000,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0006</t>
+          <t>FRC-HQ-SLM-C-2022-0006</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -56175,7 +56175,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0006</t>
+          <t>FRC-HQ-SLM-C-2022-0006</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -56350,7 +56350,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -56525,7 +56525,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -56700,7 +56700,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -56875,7 +56875,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -57050,7 +57050,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -57225,7 +57225,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -57400,7 +57400,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -57575,7 +57575,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -57750,7 +57750,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -57925,7 +57925,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -58100,7 +58100,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -58275,7 +58275,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-dfsdaf-SLM-C-2023-0001</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -58450,7 +58450,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-20-0001</t>
+          <t>FRC-HQ-SLM-T-2020-0001</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -58625,7 +58625,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-98-0000</t>
+          <t>FRC-FRC-0-C-1998-0000</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">

</xml_diff>